<commit_message>
August 31, 2020 Update
Finished Excel exporting.
</commit_message>
<xml_diff>
--- a/assets/excel/wercher_test_v2.xlsx
+++ b/assets/excel/wercher_test_v2.xlsx
@@ -29,7 +29,7 @@
     <t xml:space="preserve">Client Name:</t>
   </si>
   <si>
-    <t xml:space="preserve">B4</t>
+    <t xml:space="preserve">HELLO</t>
   </si>
   <si>
     <t xml:space="preserve">Salary Mode:</t>
@@ -221,7 +221,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>